<commit_message>
Full automation complete #3
Everything works in the automation, just needs a bit of tidying up.
</commit_message>
<xml_diff>
--- a/BlizzardAutomation/Data/Input/08072020.xlsx
+++ b/BlizzardAutomation/Data/Input/08072020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\UiPath\BlizzardAutomation\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AA9D75-B2BB-4D47-BDB0-349C5B05789D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD355D6-3A4C-4089-A89F-8FF0755041F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2250" windowWidth="23010" windowHeight="10560" activeTab="4" xr2:uid="{18BB7A54-FEA8-422E-AE54-2B010D6C4EFA}"/>
+    <workbookView xWindow="23040" yWindow="1836" windowWidth="23016" windowHeight="10560" xr2:uid="{18BB7A54-FEA8-422E-AE54-2B010D6C4EFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Monster" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
   <si>
     <t>Microsoft</t>
   </si>
@@ -59,28 +59,31 @@
     <t>Monster</t>
   </si>
   <si>
-    <t>Time (hh:mm:ss)</t>
-  </si>
-  <si>
-    <t>Open Price ($)</t>
-  </si>
-  <si>
-    <t>High Price ($)</t>
-  </si>
-  <si>
-    <t>Low Price ($)</t>
-  </si>
-  <si>
-    <t>Close Price ($)</t>
-  </si>
-  <si>
-    <t>Current Price ($)</t>
-  </si>
-  <si>
     <t>Change ($)</t>
   </si>
   <si>
     <t>Change (%)</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Price ($)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time </t>
+  </si>
+  <si>
+    <t>Open ($)</t>
+  </si>
+  <si>
+    <t>High ($)</t>
+  </si>
+  <si>
+    <t>Low ($)</t>
+  </si>
+  <si>
+    <t>Close ($)</t>
   </si>
 </sst>
 </file>
@@ -116,9 +119,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,7 +439,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34FCF8EB-2920-47C2-9AB3-C47483FB2818}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -446,28 +452,28 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="H3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -531,7 +537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B601422C-A944-4A01-9345-57B6B9528F64}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -549,7 +557,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D620EC6F-4F25-43E9-8E23-908FB75F5715}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -560,28 +570,28 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="H3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -690,6 +700,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -697,7 +708,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29E1767C-0088-44D6-BBC6-415EE0D988DC}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -708,28 +721,28 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="H3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -767,7 +780,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59ADB75-4844-4168-B8F1-638FDC6A9D80}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -778,28 +793,28 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="H3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -915,7 +930,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE8E914-43CB-49FB-ADD1-5CCB7BD5FCB6}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -925,29 +942,29 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="H3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1030,6 +1047,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>